<commit_message>
Made format for crosswalk header lines conisistent
</commit_message>
<xml_diff>
--- a/crosswalks/Geofabric-IUCNGET/Lakes-IUCNGET.xlsx
+++ b/crosswalks/Geofabric-IUCNGET/Lakes-IUCNGET.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/jor069_csiro_au/Documents/NEAP/ecosystem-typology_working-copies/crosswalks/Geofabric-IUCNGET/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/new298_csiro_au/Documents/Code/Python/NEAP/ecosystem-typology/crosswalks/Geofabric-IUCNGET/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="77" documentId="13_ncr:1_{42ACFFC3-A18D-4767-80F5-F43EBBEA0DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{453BDAF4-F7CA-4F51-839C-FC9818E50ACA}"/>
+  <xr:revisionPtr revIDLastSave="78" documentId="13_ncr:1_{42ACFFC3-A18D-4767-80F5-F43EBBEA0DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD25FAFE-63E5-486C-A234-07CFD094A101}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1995" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
+    <workbookView xWindow="4485" yWindow="2460" windowWidth="21600" windowHeight="11430" activeTab="1" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
   </bookViews>
   <sheets>
     <sheet name="header" sheetId="5" r:id="rId1"/>
@@ -37,37 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="94">
-  <si>
-    <t>subject_id</t>
-  </si>
-  <si>
-    <t>subject_label</t>
-  </si>
-  <si>
-    <t>predicate_id</t>
-  </si>
-  <si>
-    <t>object_id</t>
-  </si>
-  <si>
-    <t>object_label</t>
-  </si>
-  <si>
-    <t>mapping_justification</t>
-  </si>
-  <si>
-    <t>author_id</t>
-  </si>
-  <si>
-    <t>mapping_date</t>
-  </si>
-  <si>
-    <t>confidence</t>
-  </si>
-  <si>
-    <t>comment</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="81">
   <si>
     <t>semapv:ManualMappingCuration</t>
   </si>
@@ -75,12 +45,6 @@
     <t>skos:broadMatch</t>
   </si>
   <si>
-    <t>reviewer_id</t>
-  </si>
-  <si>
-    <t>status</t>
-  </si>
-  <si>
     <t>creator_id: https://orcid.org/0000-0002-3884-3420</t>
   </si>
   <si>
@@ -106,9 +70,6 @@
   </si>
   <si>
     <t>mapping_set_id: http://w3id.org/env/crosswalk/nesp2get/2024-02-06</t>
-  </si>
-  <si>
-    <t>author_label</t>
   </si>
   <si>
     <t>F2.1 Large permanent freshwater lakes</t>
@@ -338,18 +299,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF1F2328"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -420,18 +373,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -451,25 +398,22 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -791,64 +735,64 @@
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="104.109375" customWidth="1"/>
+    <col min="1" max="1" width="104.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -858,664 +802,698 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ACFEC63-F603-4D93-B073-540A32B07BA6}">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="34" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="34" customWidth="1"/>
-    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="68.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="68.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="7" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:14" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="6" t="s">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" s="1">
+        <v>45444</v>
+      </c>
+      <c r="K2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="7"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="L1" s="6" t="s">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" t="s">
         <v>50</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="N2" s="2"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="H3" t="s">
-        <v>63</v>
       </c>
       <c r="I3" s="1">
         <v>45444</v>
       </c>
       <c r="K3" t="s">
-        <v>36</v>
-      </c>
-      <c r="N3" s="8"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="N3" s="7"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>64</v>
+        <v>13</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="H4" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="I4" s="1">
         <v>45444</v>
       </c>
       <c r="K4" t="s">
-        <v>36</v>
-      </c>
-      <c r="N4" s="8"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="N4" s="7"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>65</v>
-      </c>
       <c r="H5" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="I5" s="1">
         <v>45444</v>
       </c>
       <c r="K5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N5" s="8"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="N5" s="7"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>83</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>80</v>
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>69</v>
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>53</v>
       </c>
       <c r="H6" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="I6" s="1">
         <v>45444</v>
       </c>
       <c r="K6" t="s">
-        <v>36</v>
-      </c>
-      <c r="N6" s="8"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="N6" s="7"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>66</v>
+        <v>15</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>54</v>
       </c>
       <c r="H7" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="I7" s="1">
         <v>45444</v>
       </c>
       <c r="K7" t="s">
-        <v>36</v>
-      </c>
-      <c r="N7" s="8"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="N7" s="7"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>67</v>
+        <v>16</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>55</v>
       </c>
       <c r="H8" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="I8" s="1">
         <v>45444</v>
       </c>
       <c r="K8" t="s">
-        <v>36</v>
-      </c>
-      <c r="N8" s="8"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="N8" s="7"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>68</v>
+        <v>39</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="H9" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="I9" s="1">
         <v>45444</v>
       </c>
       <c r="K9" t="s">
-        <v>36</v>
-      </c>
-      <c r="N9" s="8"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="N9" s="7"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" t="s">
-        <v>52</v>
+        <v>71</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>68</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>69</v>
+        <v>79</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="H10" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="I10" s="1">
         <v>45444</v>
       </c>
       <c r="K10" t="s">
-        <v>36</v>
-      </c>
-      <c r="N10" s="8"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="N10" s="7"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>81</v>
+        <v>72</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>69</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>92</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="9" t="s">
         <v>69</v>
       </c>
+      <c r="F11" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="H11" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="I11" s="1">
         <v>45444</v>
       </c>
       <c r="K11" t="s">
-        <v>36</v>
-      </c>
-      <c r="N11" s="8"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="N11" s="7"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>85</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>82</v>
+        <v>73</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>93</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>69</v>
+        <v>62</v>
+      </c>
+      <c r="E12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="H12" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="I12" s="1">
         <v>45444</v>
       </c>
       <c r="K12" t="s">
-        <v>36</v>
-      </c>
-      <c r="N12" s="8"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="N12" s="7"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="E13" t="s">
-        <v>70</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>69</v>
+        <v>58</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="H13" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="I13" s="1">
         <v>45444</v>
       </c>
       <c r="K13" t="s">
-        <v>36</v>
-      </c>
-      <c r="N13" s="8"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="N13" s="7"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="E14" t="s">
-        <v>71</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>69</v>
+        <v>59</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="H14" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="I14" s="1">
         <v>45444</v>
       </c>
       <c r="K14" t="s">
-        <v>36</v>
-      </c>
-      <c r="N14" s="8"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="N14" s="7"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="E15" t="s">
-        <v>72</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>69</v>
+        <v>60</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="H15" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="I15" s="1">
         <v>45444</v>
       </c>
       <c r="K15" t="s">
-        <v>36</v>
-      </c>
-      <c r="N15" s="8"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="N15" s="7"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E16" t="s">
-        <v>73</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>69</v>
+        <v>61</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="H16" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="I16" s="1">
         <v>45444</v>
       </c>
       <c r="K16" t="s">
-        <v>36</v>
-      </c>
-      <c r="N16" s="8"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>90</v>
-      </c>
-      <c r="B17" t="s">
-        <v>74</v>
-      </c>
-      <c r="C17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" t="s">
-        <v>79</v>
-      </c>
-      <c r="E17" t="s">
-        <v>74</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="H17" t="s">
-        <v>63</v>
-      </c>
-      <c r="I17" s="1">
-        <v>45444</v>
-      </c>
-      <c r="K17" t="s">
-        <v>36</v>
-      </c>
-      <c r="N17" s="8"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="G18" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="N16" s="7"/>
+    </row>
+    <row r="17" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G17" s="2"/>
+      <c r="I17" s="1"/>
+      <c r="N17" s="7"/>
+    </row>
+    <row r="18" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G18" s="2"/>
       <c r="I18" s="1"/>
-      <c r="N18" s="8"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="G19" s="3"/>
+      <c r="N18" s="7"/>
+    </row>
+    <row r="19" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G19" s="2"/>
       <c r="I19" s="1"/>
-      <c r="N19" s="8"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="G20" s="3"/>
+      <c r="N19" s="7"/>
+    </row>
+    <row r="20" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G20" s="2"/>
       <c r="I20" s="1"/>
-      <c r="N20" s="8"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="G21" s="3"/>
+      <c r="N20" s="7"/>
+    </row>
+    <row r="21" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G21" s="2"/>
       <c r="I21" s="1"/>
-      <c r="N21" s="8"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="G22" s="3"/>
+      <c r="N21" s="7"/>
+    </row>
+    <row r="22" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G22" s="2"/>
       <c r="I22" s="1"/>
-      <c r="N22" s="8"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="G23" s="3"/>
+      <c r="N22" s="7"/>
+    </row>
+    <row r="23" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G23" s="2"/>
       <c r="I23" s="1"/>
-      <c r="N23" s="8"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="G24" s="3"/>
+      <c r="N23" s="7"/>
+    </row>
+    <row r="24" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G24" s="2"/>
       <c r="I24" s="1"/>
-      <c r="N24" s="8"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="G25" s="3"/>
+      <c r="N24" s="7"/>
+    </row>
+    <row r="25" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G25" s="2"/>
       <c r="I25" s="1"/>
-      <c r="N25" s="8"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="G26" s="3"/>
-      <c r="I26" s="1"/>
-      <c r="N26" s="8"/>
+      <c r="N25" s="7"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="72d9be16-af35-44ba-8991-a3db737bf75a" xsi:nil="true"/>
+    <Notes0 xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a" xsi:nil="true"/>
+    <_dlc_DocId xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">63P7TJYCZHM3-28990658-16955</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">
+      <Url>https://csiroau.sharepoint.com/sites/CSIRO-LEAP/_layouts/15/DocIdRedir.aspx?ID=63P7TJYCZHM3-28990658-16955</Url>
+      <Description>63P7TJYCZHM3-28990658-16955</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100772FA3DF59B7CE49A6C16870444FDBEA" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1badbe4fae1da33fa4f3d33d98841982">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9e444dda-df07-4069-8b25-4dfb1c3da75a" xmlns:ns3="72d9be16-af35-44ba-8991-a3db737bf75a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35b20e6642ad5eb13a26fdf3049cd990" ns2:_="" ns3:_="">
     <xsd:import namespace="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
@@ -1791,83 +1769,34 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D487604F-0564-4158-A24A-3D7190C5619F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
+    <ds:schemaRef ds:uri="72d9be16-af35-44ba-8991-a3db737bf75a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC5D47B6-1317-4F93-BD6E-FCBD1047334E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="72d9be16-af35-44ba-8991-a3db737bf75a" xsi:nil="true"/>
-    <Notes0 xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a" xsi:nil="true"/>
-    <_dlc_DocId xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">63P7TJYCZHM3-28990658-16955</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">
-      <Url>https://csiroau.sharepoint.com/sites/CSIRO-LEAP/_layouts/15/DocIdRedir.aspx?ID=63P7TJYCZHM3-28990658-16955</Url>
-      <Description>63P7TJYCZHM3-28990658-16955</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39241E02-8637-4EBB-8C9C-3CF779AD8349}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66326C79-A0D3-4EA9-86BB-19E204621547}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1884,31 +1813,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39241E02-8637-4EBB-8C9C-3CF779AD8349}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC5D47B6-1317-4F93-BD6E-FCBD1047334E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D487604F-0564-4158-A24A-3D7190C5619F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
-    <ds:schemaRef ds:uri="72d9be16-af35-44ba-8991-a3db737bf75a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>